<commit_message>
Latest Kobo survey -- add notes and TODO
</commit_message>
<xml_diff>
--- a/kobo_gen_survey/Generator Survey MSRP Matchup.xlsx
+++ b/kobo_gen_survey/Generator Survey MSRP Matchup.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_UNHCR\CODE\kobo_gen_survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D3B03E-C7AB-4EC1-B011-4CF712AD6F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C268AB-81D7-4A41-BE03-95DCC9142BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3817" yWindow="3817" windowWidth="21342" windowHeight="11385" activeTab="1" xr2:uid="{33232893-FE13-C340-90F5-AE4126621A69}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="15800" xr2:uid="{33232893-FE13-C340-90F5-AE4126621A69}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="3" r:id="rId1"/>
     <sheet name="DB Tables" sheetId="4" r:id="rId2"/>
     <sheet name="msrp_survey_match" sheetId="1" r:id="rId3"/>
     <sheet name="MSRP_precloud erp.csv" sheetId="2" r:id="rId4"/>
-    <sheet name="pics_with_hrs_match_aid_msrp" sheetId="5" r:id="rId5"/>
+    <sheet name="controller_pics_nanonets" sheetId="5" r:id="rId5"/>
+    <sheet name="controller_pics_nanonets hrs" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6374" uniqueCount="2278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6699" uniqueCount="2290">
   <si>
     <t>survey_index</t>
   </si>
@@ -14858,9 +14859,6 @@
     <t>DB Tables</t>
   </si>
   <si>
-    <t>SQL to make local Tables from msrp, survaey, and ocr data</t>
-  </si>
-  <si>
     <r>
       <t>drop</t>
     </r>
@@ -17985,13 +17983,463 @@
   </si>
   <si>
     <t>SQL from Adam to get matches between survey and msrp data --- does not use runtime hrs</t>
+  </si>
+  <si>
+    <t>SQL to make local Tables from msrp, survey, and ocr data</t>
+  </si>
+  <si>
+    <t>Total Survey responses</t>
+  </si>
+  <si>
+    <t>Total Generators Pre ERP</t>
+  </si>
+  <si>
+    <t>E:\_UNHCR\CODE\kobo_gen_survey\MSRP_precloud erp.csv</t>
+  </si>
+  <si>
+    <t>Total (usable) Survey controller photos</t>
+  </si>
+  <si>
+    <t>Total controller photos with usable runtime</t>
+  </si>
+  <si>
+    <t>Total survey to Pre ERP ID matches</t>
+  </si>
+  <si>
+    <t>Total Survey controller photos ID matches</t>
+  </si>
+  <si>
+    <r>
+      <t>select</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.* </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>from</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>survey_controller_data_from_photos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>msrp_precloud_erp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>where</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>asset_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"TAG_NUMBER"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>asset_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"ASSET_NUMBER"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF800000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>asset_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF8E00C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006464"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"MSRP_ASSET_ID"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF808080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>-- 3 -- m."ASSET_NUMBER" -- 3</t>
+    </r>
+  </si>
+  <si>
+    <t>"UNHCRnnONttOIL</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>Validate reasonableness of runtime with purchase date</t>
+  </si>
+  <si>
+    <t>Validate generator kVa with between erp and survey and or on the ground personel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -18146,6 +18594,14 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -18212,7 +18668,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -18246,9 +18702,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -18267,6 +18720,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18650,15 +19107,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0ED24ED-938D-465B-B254-B2796A733D41}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.3" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="1" max="1" width="38.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -18666,7 +19123,7 @@
         <v>2217</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>2218</v>
+        <v>2277</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -18729,9 +19186,82 @@
         <v>602</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
         <v>603</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>2279</v>
+      </c>
+      <c r="B20">
+        <v>3448</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>2278</v>
+      </c>
+      <c r="B21">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>2283</v>
+      </c>
+      <c r="B22">
+        <v>469</v>
+      </c>
+      <c r="E22" t="str">
+        <f>A4</f>
+        <v>msrp_survey_match</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>2281</v>
+      </c>
+      <c r="B23">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>2284</v>
+      </c>
+      <c r="B24">
+        <v>69</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>2285</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>2282</v>
+      </c>
+      <c r="B25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30.6" x14ac:dyDescent="0.5">
+      <c r="A27" s="20" t="s">
+        <v>2287</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>2288</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>2289</v>
       </c>
     </row>
   </sheetData>
@@ -18743,7 +19273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D455D5ED-192B-40CC-AE6B-2999E35FDF7E}">
   <dimension ref="A1:AZ79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -18769,17 +19299,17 @@
       <c r="Z1" t="s">
         <v>724</v>
       </c>
-      <c r="AI1" s="15" t="s">
-        <v>2219</v>
+      <c r="AI1" s="14" t="s">
+        <v>2218</v>
       </c>
       <c r="AM1" t="s">
+        <v>2243</v>
+      </c>
+      <c r="AS1" s="8" t="s">
         <v>2244</v>
       </c>
-      <c r="AS1" s="8" t="s">
-        <v>2245</v>
-      </c>
       <c r="AZ1" t="s">
-        <v>2277</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.3">
@@ -18789,9 +19319,9 @@
       <c r="Z2" t="s">
         <v>728</v>
       </c>
-      <c r="AI2" s="16"/>
-      <c r="AS2" s="18" t="s">
-        <v>2246</v>
+      <c r="AI2" s="15"/>
+      <c r="AS2" s="17" t="s">
+        <v>2245</v>
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.3">
@@ -18804,22 +19334,22 @@
       <c r="U3" s="10" t="s">
         <v>605</v>
       </c>
-      <c r="AI3" s="15" t="s">
-        <v>2220</v>
+      <c r="AI3" s="14" t="s">
+        <v>2219</v>
       </c>
       <c r="AS3" s="9" t="s">
-        <v>2247</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="I4" s="11"/>
       <c r="U4" s="11"/>
-      <c r="AI4" s="15" t="s">
-        <v>2221</v>
+      <c r="AI4" s="14" t="s">
+        <v>2220</v>
       </c>
       <c r="AS4" s="9" t="s">
-        <v>2248</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.3">
@@ -18832,22 +19362,22 @@
       <c r="U5" s="10" t="s">
         <v>650</v>
       </c>
-      <c r="AI5" s="15" t="s">
-        <v>2222</v>
+      <c r="AI5" s="14" t="s">
+        <v>2221</v>
       </c>
       <c r="AS5" s="9" t="s">
-        <v>2249</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="I6" s="11"/>
       <c r="U6" s="11"/>
-      <c r="AI6" s="17" t="s">
-        <v>2223</v>
+      <c r="AI6" s="16" t="s">
+        <v>2222</v>
       </c>
       <c r="AS6" s="9" t="s">
-        <v>2250</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.3">
@@ -18860,11 +19390,11 @@
       <c r="U7" s="8" t="s">
         <v>651</v>
       </c>
-      <c r="AI7" s="17" t="s">
-        <v>2224</v>
+      <c r="AI7" s="16" t="s">
+        <v>2223</v>
       </c>
       <c r="AS7" s="9" t="s">
-        <v>2251</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.3">
@@ -18877,11 +19407,11 @@
       <c r="U8" s="12" t="s">
         <v>652</v>
       </c>
-      <c r="AI8" s="17" t="s">
-        <v>2225</v>
+      <c r="AI8" s="16" t="s">
+        <v>2224</v>
       </c>
       <c r="AS8" s="9" t="s">
-        <v>2252</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.3">
@@ -18894,11 +19424,11 @@
       <c r="U9" s="12" t="s">
         <v>653</v>
       </c>
-      <c r="AI9" s="17" t="s">
-        <v>2226</v>
+      <c r="AI9" s="16" t="s">
+        <v>2225</v>
       </c>
       <c r="AS9" s="9" t="s">
-        <v>2253</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.3">
@@ -18911,11 +19441,11 @@
       <c r="U10" s="12" t="s">
         <v>654</v>
       </c>
-      <c r="AI10" s="17" t="s">
-        <v>2227</v>
+      <c r="AI10" s="16" t="s">
+        <v>2226</v>
       </c>
       <c r="AS10" s="9" t="s">
-        <v>2254</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.3">
@@ -18928,11 +19458,11 @@
       <c r="U11" s="12" t="s">
         <v>655</v>
       </c>
-      <c r="AI11" s="17" t="s">
-        <v>2228</v>
+      <c r="AI11" s="16" t="s">
+        <v>2227</v>
       </c>
       <c r="AS11" s="9" t="s">
-        <v>2255</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.3">
@@ -18945,11 +19475,11 @@
       <c r="U12" s="12" t="s">
         <v>656</v>
       </c>
-      <c r="AI12" s="17" t="s">
-        <v>2229</v>
+      <c r="AI12" s="16" t="s">
+        <v>2228</v>
       </c>
       <c r="AS12" s="9" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.3">
@@ -18962,11 +19492,11 @@
       <c r="U13" s="12" t="s">
         <v>657</v>
       </c>
-      <c r="AI13" s="17" t="s">
-        <v>2230</v>
+      <c r="AI13" s="16" t="s">
+        <v>2229</v>
       </c>
       <c r="AS13" s="9" t="s">
-        <v>2257</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.3">
@@ -18979,11 +19509,11 @@
       <c r="U14" s="12" t="s">
         <v>658</v>
       </c>
-      <c r="AI14" s="17" t="s">
-        <v>2231</v>
+      <c r="AI14" s="16" t="s">
+        <v>2230</v>
       </c>
       <c r="AS14" s="9" t="s">
-        <v>2258</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="15" spans="1:52" x14ac:dyDescent="0.3">
@@ -18996,11 +19526,11 @@
       <c r="U15" s="12" t="s">
         <v>659</v>
       </c>
-      <c r="AI15" s="17" t="s">
-        <v>2232</v>
+      <c r="AI15" s="16" t="s">
+        <v>2231</v>
       </c>
       <c r="AS15" s="9" t="s">
-        <v>2259</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.3">
@@ -19013,11 +19543,11 @@
       <c r="U16" s="12" t="s">
         <v>660</v>
       </c>
-      <c r="AI16" s="17" t="s">
-        <v>2233</v>
+      <c r="AI16" s="16" t="s">
+        <v>2232</v>
       </c>
       <c r="AS16" s="8" t="s">
-        <v>2260</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="17" spans="1:45" x14ac:dyDescent="0.3">
@@ -19030,11 +19560,11 @@
       <c r="U17" s="12" t="s">
         <v>661</v>
       </c>
-      <c r="AI17" s="17" t="s">
-        <v>2234</v>
+      <c r="AI17" s="16" t="s">
+        <v>2233</v>
       </c>
       <c r="AS17" s="8" t="s">
-        <v>2261</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="18" spans="1:45" x14ac:dyDescent="0.3">
@@ -19044,11 +19574,11 @@
       <c r="U18" s="12" t="s">
         <v>662</v>
       </c>
-      <c r="AI18" s="17" t="s">
-        <v>2235</v>
-      </c>
-      <c r="AS18" s="19" t="s">
-        <v>2262</v>
+      <c r="AI18" s="16" t="s">
+        <v>2234</v>
+      </c>
+      <c r="AS18" s="18" t="s">
+        <v>2261</v>
       </c>
     </row>
     <row r="19" spans="1:45" x14ac:dyDescent="0.3">
@@ -19058,11 +19588,11 @@
       <c r="U19" s="12" t="s">
         <v>663</v>
       </c>
-      <c r="AI19" s="17" t="s">
-        <v>2236</v>
+      <c r="AI19" s="16" t="s">
+        <v>2235</v>
       </c>
       <c r="AS19" s="9" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="20" spans="1:45" x14ac:dyDescent="0.3">
@@ -19075,11 +19605,11 @@
       <c r="U20" s="12" t="s">
         <v>664</v>
       </c>
-      <c r="AI20" s="17" t="s">
-        <v>2237</v>
+      <c r="AI20" s="16" t="s">
+        <v>2236</v>
       </c>
       <c r="AS20" s="9" t="s">
-        <v>2264</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="21" spans="1:45" x14ac:dyDescent="0.3">
@@ -19092,11 +19622,11 @@
       <c r="U21" s="12" t="s">
         <v>665</v>
       </c>
-      <c r="AI21" s="17" t="s">
-        <v>2238</v>
+      <c r="AI21" s="16" t="s">
+        <v>2237</v>
       </c>
       <c r="AS21" s="9" t="s">
-        <v>2265</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="22" spans="1:45" x14ac:dyDescent="0.3">
@@ -19109,11 +19639,11 @@
       <c r="U22" s="12" t="s">
         <v>666</v>
       </c>
-      <c r="AI22" s="17" t="s">
-        <v>2239</v>
+      <c r="AI22" s="16" t="s">
+        <v>2238</v>
       </c>
       <c r="AS22" s="9" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="23" spans="1:45" x14ac:dyDescent="0.3">
@@ -19123,11 +19653,11 @@
       <c r="U23" s="12" t="s">
         <v>667</v>
       </c>
-      <c r="AI23" s="17" t="s">
-        <v>2240</v>
+      <c r="AI23" s="16" t="s">
+        <v>2239</v>
       </c>
       <c r="AS23" s="9" t="s">
-        <v>2267</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="24" spans="1:45" x14ac:dyDescent="0.3">
@@ -19140,11 +19670,11 @@
       <c r="U24" s="12" t="s">
         <v>668</v>
       </c>
-      <c r="AI24" s="17" t="s">
-        <v>2241</v>
+      <c r="AI24" s="16" t="s">
+        <v>2240</v>
       </c>
       <c r="AS24" s="9" t="s">
-        <v>2268</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="25" spans="1:45" x14ac:dyDescent="0.3">
@@ -19154,11 +19684,11 @@
       <c r="U25" s="12" t="s">
         <v>669</v>
       </c>
-      <c r="AI25" s="17" t="s">
-        <v>2242</v>
+      <c r="AI25" s="16" t="s">
+        <v>2241</v>
       </c>
       <c r="AS25" s="9" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="26" spans="1:45" x14ac:dyDescent="0.3">
@@ -19168,11 +19698,11 @@
       <c r="U26" s="12" t="s">
         <v>670</v>
       </c>
-      <c r="AI26" s="15" t="s">
-        <v>2243</v>
+      <c r="AI26" s="14" t="s">
+        <v>2242</v>
       </c>
       <c r="AS26" s="9" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
     </row>
     <row r="27" spans="1:45" x14ac:dyDescent="0.3">
@@ -19183,7 +19713,7 @@
         <v>671</v>
       </c>
       <c r="AS27" s="8" t="s">
-        <v>2271</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="28" spans="1:45" x14ac:dyDescent="0.3">
@@ -19194,7 +19724,7 @@
         <v>672</v>
       </c>
       <c r="AS28" s="8" t="s">
-        <v>2272</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="29" spans="1:45" x14ac:dyDescent="0.3">
@@ -19205,7 +19735,7 @@
         <v>673</v>
       </c>
       <c r="AS29" s="8" t="s">
-        <v>2273</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="30" spans="1:45" x14ac:dyDescent="0.3">
@@ -19216,7 +19746,7 @@
         <v>674</v>
       </c>
       <c r="AS30" s="8" t="s">
-        <v>2274</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="31" spans="1:45" x14ac:dyDescent="0.3">
@@ -19227,7 +19757,7 @@
         <v>675</v>
       </c>
       <c r="AS31" s="8" t="s">
-        <v>2275</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="32" spans="1:45" x14ac:dyDescent="0.3">
@@ -19238,7 +19768,7 @@
         <v>676</v>
       </c>
       <c r="AS32" s="8" t="s">
-        <v>2276</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="33" spans="9:21" x14ac:dyDescent="0.3">
@@ -19540,10 +20070,10 @@
       <c r="C5" s="6" t="s">
         <v>472</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="19" t="s">
         <v>471</v>
       </c>
-      <c r="E5" s="13"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C6" s="5">
@@ -49328,7 +49858,7 @@
   <dimension ref="A1:I388"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A382" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -49379,7 +49909,7 @@
       <c r="E2">
         <v>1083</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>742</v>
       </c>
       <c r="G2" t="s">
@@ -49529,7 +50059,7 @@
       <c r="D8" t="s">
         <v>766</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>767</v>
       </c>
     </row>
@@ -49590,7 +50120,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="228.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="130.44999999999999" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>781</v>
       </c>
@@ -49606,7 +50136,7 @@
       <c r="E12">
         <v>2117</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="13" t="s">
         <v>784</v>
       </c>
       <c r="G12" t="s">
@@ -49740,7 +50270,7 @@
         <v>5122</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="130.44999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="97.85" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>811</v>
       </c>
@@ -49753,7 +50283,7 @@
       <c r="D18" t="s">
         <v>813</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="13" t="s">
         <v>814</v>
       </c>
       <c r="G18" t="s">
@@ -49859,7 +50389,7 @@
       <c r="D23" t="s">
         <v>836</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="13" t="s">
         <v>837</v>
       </c>
     </row>
@@ -50427,7 +50957,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="358.65" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="293.45" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>947</v>
       </c>
@@ -50440,7 +50970,7 @@
       <c r="D48" t="s">
         <v>949</v>
       </c>
-      <c r="F48" s="14" t="s">
+      <c r="F48" s="13" t="s">
         <v>950</v>
       </c>
       <c r="G48" t="s">
@@ -50550,7 +51080,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="130.44999999999999" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="114.15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>968</v>
       </c>
@@ -50563,7 +51093,7 @@
       <c r="D54" t="s">
         <v>970</v>
       </c>
-      <c r="F54" s="14" t="s">
+      <c r="F54" s="13" t="s">
         <v>971</v>
       </c>
     </row>
@@ -50863,7 +51393,7 @@
         <v>431174</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="146.75" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="48.9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>739</v>
       </c>
@@ -50879,7 +51409,7 @@
       <c r="E71">
         <v>1083</v>
       </c>
-      <c r="F71" s="14" t="s">
+      <c r="F71" s="13" t="s">
         <v>1039</v>
       </c>
       <c r="G71" t="s">
@@ -51006,7 +51536,7 @@
       <c r="D76" t="s">
         <v>1049</v>
       </c>
-      <c r="F76" s="14" t="s">
+      <c r="F76" s="13" t="s">
         <v>1050</v>
       </c>
     </row>
@@ -51056,7 +51586,7 @@
         <v>3484</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="228.25" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="130.44999999999999" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>781</v>
       </c>
@@ -51072,7 +51602,7 @@
       <c r="E79">
         <v>2117</v>
       </c>
-      <c r="F79" s="14" t="s">
+      <c r="F79" s="13" t="s">
         <v>784</v>
       </c>
       <c r="G79" t="s">
@@ -51229,7 +51759,7 @@
         <v>5122</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="130.44999999999999" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="97.85" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>811</v>
       </c>
@@ -51242,7 +51772,7 @@
       <c r="D86" t="s">
         <v>1071</v>
       </c>
-      <c r="F86" s="14" t="s">
+      <c r="F86" s="13" t="s">
         <v>814</v>
       </c>
       <c r="G86" t="s">
@@ -51348,7 +51878,7 @@
       <c r="D91" t="s">
         <v>1083</v>
       </c>
-      <c r="F91" s="14" t="s">
+      <c r="F91" s="13" t="s">
         <v>1084</v>
       </c>
     </row>
@@ -51421,7 +51951,7 @@
         <v>1102.3</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="374.95" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="179.35" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>850</v>
       </c>
@@ -51434,7 +51964,7 @@
       <c r="D95" t="s">
         <v>1092</v>
       </c>
-      <c r="F95" s="14" t="s">
+      <c r="F95" s="13" t="s">
         <v>1093</v>
       </c>
       <c r="G95" t="s">
@@ -51444,7 +51974,7 @@
         <v>1300.3</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="211.95" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="114.15" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>854</v>
       </c>
@@ -51457,7 +51987,7 @@
       <c r="D96" t="s">
         <v>1096</v>
       </c>
-      <c r="F96" s="14" t="s">
+      <c r="F96" s="13" t="s">
         <v>1097</v>
       </c>
       <c r="G96">
@@ -52137,7 +52667,7 @@
         <v>5159</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="211.95" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" ht="130.44999999999999" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>1185</v>
       </c>
@@ -52153,7 +52683,7 @@
       <c r="E126">
         <v>2103</v>
       </c>
-      <c r="F126" s="14" t="s">
+      <c r="F126" s="13" t="s">
         <v>1188</v>
       </c>
       <c r="G126" t="s">
@@ -52189,7 +52719,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" ht="211.95" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>1195</v>
       </c>
@@ -52205,7 +52735,7 @@
       <c r="E128">
         <v>1113</v>
       </c>
-      <c r="F128" s="14" t="s">
+      <c r="F128" s="13" t="s">
         <v>1198</v>
       </c>
       <c r="G128" t="s">
@@ -52228,7 +52758,7 @@
       <c r="D129" t="s">
         <v>1202</v>
       </c>
-      <c r="F129" s="14" t="s">
+      <c r="F129" s="13" t="s">
         <v>1203</v>
       </c>
       <c r="G129" t="s">
@@ -52290,7 +52820,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="114.15" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" ht="48.9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>1215</v>
       </c>
@@ -52306,7 +52836,7 @@
       <c r="E132">
         <v>1040</v>
       </c>
-      <c r="F132" s="14" t="s">
+      <c r="F132" s="13" t="s">
         <v>1218</v>
       </c>
       <c r="G132" t="s">
@@ -52379,7 +52909,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="309.75" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" ht="163.05000000000001" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>1232</v>
       </c>
@@ -52392,7 +52922,7 @@
       <c r="D136" t="s">
         <v>1234</v>
       </c>
-      <c r="F136" s="14" t="s">
+      <c r="F136" s="13" t="s">
         <v>1235</v>
       </c>
       <c r="G136">
@@ -52477,7 +53007,7 @@
         <v>4330</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" ht="293.45" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>1250</v>
       </c>
@@ -52493,7 +53023,7 @@
       <c r="E140">
         <v>1535</v>
       </c>
-      <c r="F140" s="14" t="s">
+      <c r="F140" s="13" t="s">
         <v>1253</v>
       </c>
       <c r="G140">
@@ -52503,7 +53033,7 @@
         <v>4700.1000000000004</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" ht="260.85000000000002" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>1254</v>
       </c>
@@ -52519,7 +53049,7 @@
       <c r="E141">
         <v>2270</v>
       </c>
-      <c r="F141" s="14" t="s">
+      <c r="F141" s="13" t="s">
         <v>1257</v>
       </c>
       <c r="G141" t="s">
@@ -52529,7 +53059,7 @@
         <v>4736</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" ht="228.25" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>1259</v>
       </c>
@@ -52545,7 +53075,7 @@
       <c r="E142">
         <v>1487</v>
       </c>
-      <c r="F142" s="14" t="s">
+      <c r="F142" s="13" t="s">
         <v>1262</v>
       </c>
       <c r="G142">
@@ -52678,7 +53208,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" ht="309.75" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>1290</v>
       </c>
@@ -52691,7 +53221,7 @@
       <c r="D149" t="s">
         <v>1292</v>
       </c>
-      <c r="F149" s="14" t="s">
+      <c r="F149" s="13" t="s">
         <v>1293</v>
       </c>
     </row>
@@ -52741,7 +53271,7 @@
         <v>4274</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="81.55" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" ht="48.9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>1303</v>
       </c>
@@ -52754,7 +53284,7 @@
       <c r="D152" t="s">
         <v>1305</v>
       </c>
-      <c r="F152" s="14" t="s">
+      <c r="F152" s="13" t="s">
         <v>1306</v>
       </c>
       <c r="G152">
@@ -52797,7 +53327,7 @@
       <c r="D154" t="s">
         <v>1313</v>
       </c>
-      <c r="F154" s="14" t="s">
+      <c r="F154" s="13" t="s">
         <v>1314</v>
       </c>
       <c r="G154">
@@ -52807,7 +53337,7 @@
         <v>2857</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="195.65" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" ht="97.85" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>1315</v>
       </c>
@@ -52820,7 +53350,7 @@
       <c r="D155" t="s">
         <v>1317</v>
       </c>
-      <c r="F155" s="14" t="s">
+      <c r="F155" s="13" t="s">
         <v>1318</v>
       </c>
       <c r="G155">
@@ -52847,7 +53377,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="407.55" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" ht="228.25" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>1323</v>
       </c>
@@ -52863,7 +53393,7 @@
       <c r="E157">
         <v>2578</v>
       </c>
-      <c r="F157" s="14" t="s">
+      <c r="F157" s="13" t="s">
         <v>1326</v>
       </c>
       <c r="G157">
@@ -53048,7 +53578,7 @@
         <v>3134</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" ht="244.55" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>1361</v>
       </c>
@@ -53064,7 +53594,7 @@
       <c r="E166">
         <v>1063</v>
       </c>
-      <c r="F166" s="14" t="s">
+      <c r="F166" s="13" t="s">
         <v>1364</v>
       </c>
       <c r="G166">
@@ -53462,7 +53992,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="184" spans="1:9" ht="114.15" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" ht="48.9" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>1442</v>
       </c>
@@ -53478,7 +54008,7 @@
       <c r="E184">
         <v>966</v>
       </c>
-      <c r="F184" s="14" t="s">
+      <c r="F184" s="13" t="s">
         <v>1445</v>
       </c>
       <c r="G184" t="s">
@@ -53541,7 +54071,7 @@
       <c r="D187" t="s">
         <v>1457</v>
       </c>
-      <c r="F187" s="14" t="s">
+      <c r="F187" s="13" t="s">
         <v>1458</v>
       </c>
       <c r="G187" t="s">
@@ -53551,7 +54081,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="188" spans="1:9" ht="130.44999999999999" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" ht="65.25" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>1460</v>
       </c>
@@ -53567,7 +54097,7 @@
       <c r="E188">
         <v>281</v>
       </c>
-      <c r="F188" s="14" t="s">
+      <c r="F188" s="13" t="s">
         <v>1463</v>
       </c>
       <c r="G188" t="s">
@@ -53577,7 +54107,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="189" spans="1:9" ht="163.05000000000001" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" ht="97.85" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>1465</v>
       </c>
@@ -53590,7 +54120,7 @@
       <c r="D189" t="s">
         <v>1467</v>
       </c>
-      <c r="F189" s="14" t="s">
+      <c r="F189" s="13" t="s">
         <v>1468</v>
       </c>
       <c r="G189" t="s">
@@ -53766,7 +54296,7 @@
         <v>18089</v>
       </c>
     </row>
-    <row r="198" spans="1:9" ht="260.85000000000002" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" ht="130.44999999999999" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>1505</v>
       </c>
@@ -53782,7 +54312,7 @@
       <c r="E198">
         <v>291</v>
       </c>
-      <c r="F198" s="14" t="s">
+      <c r="F198" s="13" t="s">
         <v>1508</v>
       </c>
       <c r="G198">
@@ -53818,7 +54348,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="200" spans="1:9" ht="146.75" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" ht="114.15" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>1513</v>
       </c>
@@ -53831,7 +54361,7 @@
       <c r="D200" t="s">
         <v>1515</v>
       </c>
-      <c r="F200" s="14" t="s">
+      <c r="F200" s="13" t="s">
         <v>1516</v>
       </c>
     </row>
@@ -53915,7 +54445,7 @@
         <v>864550</v>
       </c>
     </row>
-    <row r="205" spans="1:9" ht="342.35" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" ht="228.25" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>1534</v>
       </c>
@@ -53928,7 +54458,7 @@
       <c r="D205" t="s">
         <v>1536</v>
       </c>
-      <c r="F205" s="14" t="s">
+      <c r="F205" s="13" t="s">
         <v>1537</v>
       </c>
       <c r="G205" t="s">
@@ -54221,7 +54751,7 @@
         <v>776486</v>
       </c>
     </row>
-    <row r="220" spans="1:9" ht="342.35" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" ht="211.95" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>1596</v>
       </c>
@@ -54234,7 +54764,7 @@
       <c r="D220" t="s">
         <v>1598</v>
       </c>
-      <c r="F220" s="14" t="s">
+      <c r="F220" s="13" t="s">
         <v>1599</v>
       </c>
     </row>
@@ -54255,7 +54785,7 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" ht="293.45" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>1604</v>
       </c>
@@ -54268,7 +54798,7 @@
       <c r="D222" t="s">
         <v>1606</v>
       </c>
-      <c r="F222" s="14" t="s">
+      <c r="F222" s="13" t="s">
         <v>1607</v>
       </c>
     </row>
@@ -54344,7 +54874,7 @@
         <v>6118</v>
       </c>
     </row>
-    <row r="226" spans="1:9" ht="97.85" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" ht="65.25" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>1623</v>
       </c>
@@ -54357,7 +54887,7 @@
       <c r="D226" t="s">
         <v>1625</v>
       </c>
-      <c r="F226" s="14" t="s">
+      <c r="F226" s="13" t="s">
         <v>1626</v>
       </c>
       <c r="G226">
@@ -54416,7 +54946,7 @@
         <v>4270</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="195.65" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" ht="97.85" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>1637</v>
       </c>
@@ -54432,7 +54962,7 @@
       <c r="E229">
         <v>674</v>
       </c>
-      <c r="F229" s="14" t="s">
+      <c r="F229" s="13" t="s">
         <v>1640</v>
       </c>
       <c r="G229" t="s">
@@ -54600,7 +55130,7 @@
         <v>7951</v>
       </c>
     </row>
-    <row r="237" spans="1:9" ht="114.15" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9" ht="48.9" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>1673</v>
       </c>
@@ -54616,7 +55146,7 @@
       <c r="E237">
         <v>502</v>
       </c>
-      <c r="F237" s="14" t="s">
+      <c r="F237" s="13" t="s">
         <v>1676</v>
       </c>
       <c r="G237" t="s">
@@ -54724,7 +55254,7 @@
         <v>2998</v>
       </c>
     </row>
-    <row r="242" spans="1:9" ht="48.9" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:9" ht="32.6" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>1698</v>
       </c>
@@ -54737,7 +55267,7 @@
       <c r="D242" t="s">
         <v>1700</v>
       </c>
-      <c r="F242" s="14" t="s">
+      <c r="F242" s="13" t="s">
         <v>1701</v>
       </c>
       <c r="G242" t="s">
@@ -54747,7 +55277,7 @@
         <v>14440</v>
       </c>
     </row>
-    <row r="243" spans="1:9" ht="114.15" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:9" ht="48.9" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>1703</v>
       </c>
@@ -54763,7 +55293,7 @@
       <c r="E243">
         <v>1346</v>
       </c>
-      <c r="F243" s="14" t="s">
+      <c r="F243" s="13" t="s">
         <v>1706</v>
       </c>
       <c r="G243" t="s">
@@ -54773,7 +55303,7 @@
         <v>2530</v>
       </c>
     </row>
-    <row r="244" spans="1:9" ht="130.44999999999999" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9" ht="48.9" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>1708</v>
       </c>
@@ -54789,7 +55319,7 @@
       <c r="E244">
         <v>820</v>
       </c>
-      <c r="F244" s="14" t="s">
+      <c r="F244" s="13" t="s">
         <v>1711</v>
       </c>
       <c r="G244" t="s">
@@ -54874,7 +55404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="248" spans="1:9" ht="114.15" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9" ht="48.9" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>1727</v>
       </c>
@@ -54890,7 +55420,7 @@
       <c r="E248">
         <v>1162</v>
       </c>
-      <c r="F248" s="14" t="s">
+      <c r="F248" s="13" t="s">
         <v>1730</v>
       </c>
       <c r="G248" t="s">
@@ -55058,7 +55588,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="256" spans="1:9" ht="130.44999999999999" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:9" ht="81.55" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>1764</v>
       </c>
@@ -55071,11 +55601,11 @@
       <c r="D256" t="s">
         <v>1766</v>
       </c>
-      <c r="F256" s="14" t="s">
+      <c r="F256" s="13" t="s">
         <v>1767</v>
       </c>
     </row>
-    <row r="257" spans="1:9" ht="244.55" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" ht="179.35" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>1768</v>
       </c>
@@ -55088,7 +55618,7 @@
       <c r="D257" t="s">
         <v>1770</v>
       </c>
-      <c r="F257" s="14" t="s">
+      <c r="F257" s="13" t="s">
         <v>1771</v>
       </c>
       <c r="G257" t="s">
@@ -55115,7 +55645,7 @@
         <v>1776</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="48.9" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:9" ht="32.6" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>1777</v>
       </c>
@@ -55128,11 +55658,11 @@
       <c r="D259" t="s">
         <v>1779</v>
       </c>
-      <c r="F259" s="14" t="s">
+      <c r="F259" s="13" t="s">
         <v>1780</v>
       </c>
     </row>
-    <row r="260" spans="1:9" ht="293.45" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:9" ht="179.35" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>1781</v>
       </c>
@@ -55145,7 +55675,7 @@
       <c r="D260" t="s">
         <v>1783</v>
       </c>
-      <c r="F260" s="14" t="s">
+      <c r="F260" s="13" t="s">
         <v>1784</v>
       </c>
     </row>
@@ -55212,7 +55742,7 @@
         <v>9439</v>
       </c>
     </row>
-    <row r="264" spans="1:9" ht="244.55" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:9" ht="146.75" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>1799</v>
       </c>
@@ -55225,7 +55755,7 @@
       <c r="D264" t="s">
         <v>1801</v>
       </c>
-      <c r="F264" s="14" t="s">
+      <c r="F264" s="13" t="s">
         <v>1802</v>
       </c>
     </row>
@@ -55263,7 +55793,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="267" spans="1:9" ht="146.75" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:9" ht="114.15" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>1811</v>
       </c>
@@ -55276,7 +55806,7 @@
       <c r="D267" t="s">
         <v>1813</v>
       </c>
-      <c r="F267" s="14" t="s">
+      <c r="F267" s="13" t="s">
         <v>1814</v>
       </c>
     </row>
@@ -55323,7 +55853,7 @@
         <v>107.72</v>
       </c>
     </row>
-    <row r="270" spans="1:9" ht="228.25" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:9" ht="114.15" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>1822</v>
       </c>
@@ -55336,7 +55866,7 @@
       <c r="D270" t="s">
         <v>1824</v>
       </c>
-      <c r="F270" s="14" t="s">
+      <c r="F270" s="13" t="s">
         <v>1825</v>
       </c>
     </row>
@@ -55386,7 +55916,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="273" spans="1:9" ht="48.9" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:9" ht="32.6" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>1835</v>
       </c>
@@ -55399,7 +55929,7 @@
       <c r="D273" t="s">
         <v>1837</v>
       </c>
-      <c r="F273" s="14" t="s">
+      <c r="F273" s="13" t="s">
         <v>1838</v>
       </c>
       <c r="G273">
@@ -55458,7 +55988,7 @@
         <v>3036.3</v>
       </c>
     </row>
-    <row r="276" spans="1:9" ht="211.95" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9" ht="114.15" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>1848</v>
       </c>
@@ -55474,7 +56004,7 @@
       <c r="E276">
         <v>2024</v>
       </c>
-      <c r="F276" s="14" t="s">
+      <c r="F276" s="13" t="s">
         <v>1851</v>
       </c>
       <c r="G276" t="s">
@@ -55504,7 +56034,7 @@
         <v>802791</v>
       </c>
     </row>
-    <row r="278" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:9" ht="228.25" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>1857</v>
       </c>
@@ -55517,7 +56047,7 @@
       <c r="D278" t="s">
         <v>1859</v>
       </c>
-      <c r="F278" s="14" t="s">
+      <c r="F278" s="13" t="s">
         <v>1860</v>
       </c>
       <c r="G278">
@@ -55527,7 +56057,7 @@
         <v>604.9</v>
       </c>
     </row>
-    <row r="279" spans="1:9" ht="179.35" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9" ht="97.85" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>1861</v>
       </c>
@@ -55543,7 +56073,7 @@
       <c r="E279">
         <v>183</v>
       </c>
-      <c r="F279" s="14" t="s">
+      <c r="F279" s="13" t="s">
         <v>1864</v>
       </c>
       <c r="G279" t="s">
@@ -55826,7 +56356,7 @@
         <v>71.7</v>
       </c>
     </row>
-    <row r="292" spans="1:9" ht="326.05" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:9" ht="163.05000000000001" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>1919</v>
       </c>
@@ -55839,7 +56369,7 @@
       <c r="D292" t="s">
         <v>1921</v>
       </c>
-      <c r="F292" s="14" t="s">
+      <c r="F292" s="13" t="s">
         <v>1922</v>
       </c>
     </row>
@@ -56083,7 +56613,7 @@
         <v>776486</v>
       </c>
     </row>
-    <row r="305" spans="1:9" ht="342.35" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:9" ht="211.95" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>1596</v>
       </c>
@@ -56096,11 +56626,11 @@
       <c r="D305" t="s">
         <v>1960</v>
       </c>
-      <c r="F305" s="14" t="s">
+      <c r="F305" s="13" t="s">
         <v>1599</v>
       </c>
     </row>
-    <row r="306" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:9" ht="277.14999999999998" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>1604</v>
       </c>
@@ -56113,7 +56643,7 @@
       <c r="D306" t="s">
         <v>1962</v>
       </c>
-      <c r="F306" s="14" t="s">
+      <c r="F306" s="13" t="s">
         <v>1963</v>
       </c>
     </row>
@@ -56393,7 +56923,7 @@
         <v>639255</v>
       </c>
     </row>
-    <row r="319" spans="1:9" ht="195.65" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:9" ht="97.85" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>2004</v>
       </c>
@@ -56406,7 +56936,7 @@
       <c r="D319" t="s">
         <v>2006</v>
       </c>
-      <c r="F319" s="14" t="s">
+      <c r="F319" s="13" t="s">
         <v>2007</v>
       </c>
       <c r="G319">
@@ -56433,7 +56963,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="321" spans="1:8" ht="391.25" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:8" ht="211.95" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>1919</v>
       </c>
@@ -56446,7 +56976,7 @@
       <c r="D321" t="s">
         <v>2012</v>
       </c>
-      <c r="F321" s="14" t="s">
+      <c r="F321" s="13" t="s">
         <v>2013</v>
       </c>
     </row>
@@ -56646,7 +57176,7 @@
         <v>776486</v>
       </c>
     </row>
-    <row r="333" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:8" ht="293.45" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>1596</v>
       </c>
@@ -56659,7 +57189,7 @@
       <c r="D333" t="s">
         <v>2053</v>
       </c>
-      <c r="F333" s="14" t="s">
+      <c r="F333" s="13" t="s">
         <v>2054</v>
       </c>
     </row>
@@ -56743,7 +57273,7 @@
         <v>1622</v>
       </c>
     </row>
-    <row r="338" spans="1:7" ht="97.85" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:7" ht="65.25" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>1623</v>
       </c>
@@ -56756,7 +57286,7 @@
       <c r="D338" t="s">
         <v>2065</v>
       </c>
-      <c r="F338" s="14" t="s">
+      <c r="F338" s="13" t="s">
         <v>1626</v>
       </c>
       <c r="G338">
@@ -56806,7 +57336,7 @@
         <v>4270</v>
       </c>
     </row>
-    <row r="341" spans="1:7" ht="195.65" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:7" ht="97.85" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>1637</v>
       </c>
@@ -56822,7 +57352,7 @@
       <c r="E341">
         <v>674</v>
       </c>
-      <c r="F341" s="14" t="s">
+      <c r="F341" s="13" t="s">
         <v>2072</v>
       </c>
       <c r="G341">
@@ -56852,7 +57382,7 @@
         <v>3615</v>
       </c>
     </row>
-    <row r="343" spans="1:7" ht="130.44999999999999" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:7" ht="48.9" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>1647</v>
       </c>
@@ -56868,14 +57398,14 @@
       <c r="E343">
         <v>1071</v>
       </c>
-      <c r="F343" s="14" t="s">
+      <c r="F343" s="13" t="s">
         <v>2077</v>
       </c>
       <c r="G343">
         <v>2164</v>
       </c>
     </row>
-    <row r="344" spans="1:7" ht="244.55" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:7" ht="97.85" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>1652</v>
       </c>
@@ -56891,7 +57421,7 @@
       <c r="E344">
         <v>4258</v>
       </c>
-      <c r="F344" s="14" t="s">
+      <c r="F344" s="13" t="s">
         <v>2080</v>
       </c>
       <c r="G344">
@@ -56912,7 +57442,7 @@
         <v>2082</v>
       </c>
     </row>
-    <row r="346" spans="1:7" ht="179.35" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:7" ht="114.15" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>2083</v>
       </c>
@@ -56925,7 +57455,7 @@
       <c r="D346" t="s">
         <v>2085</v>
       </c>
-      <c r="F346" s="14" t="s">
+      <c r="F346" s="13" t="s">
         <v>2086</v>
       </c>
     </row>
@@ -57006,7 +57536,7 @@
         <v>2095</v>
       </c>
     </row>
-    <row r="351" spans="1:7" ht="244.55" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:7" ht="146.75" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>1768</v>
       </c>
@@ -57019,7 +57549,7 @@
       <c r="D351" t="s">
         <v>2097</v>
       </c>
-      <c r="F351" s="14" t="s">
+      <c r="F351" s="13" t="s">
         <v>2098</v>
       </c>
     </row>
@@ -57040,7 +57570,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="353" spans="1:8" ht="228.25" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:8" ht="114.15" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>1822</v>
       </c>
@@ -57053,11 +57583,11 @@
       <c r="D353" t="s">
         <v>2102</v>
       </c>
-      <c r="F353" s="14" t="s">
+      <c r="F353" s="13" t="s">
         <v>1825</v>
       </c>
     </row>
-    <row r="354" spans="1:8" ht="211.95" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:8" ht="130.44999999999999" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>1407</v>
       </c>
@@ -57073,7 +57603,7 @@
       <c r="E354">
         <v>1273</v>
       </c>
-      <c r="F354" s="14" t="s">
+      <c r="F354" s="13" t="s">
         <v>2105</v>
       </c>
       <c r="G354">
@@ -57109,7 +57639,7 @@
         <v>799979</v>
       </c>
     </row>
-    <row r="356" spans="1:8" ht="114.15" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:8" ht="81.55" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>1417</v>
       </c>
@@ -57122,7 +57652,7 @@
       <c r="D356" t="s">
         <v>2109</v>
       </c>
-      <c r="F356" s="14" t="s">
+      <c r="F356" s="13" t="s">
         <v>2110</v>
       </c>
       <c r="G356">
@@ -57175,7 +57705,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="359" spans="1:8" ht="114.15" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:8" ht="48.9" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>1432</v>
       </c>
@@ -57191,14 +57721,14 @@
       <c r="E359">
         <v>518</v>
       </c>
-      <c r="F359" s="14" t="s">
+      <c r="F359" s="13" t="s">
         <v>2119</v>
       </c>
       <c r="G359">
         <v>593</v>
       </c>
     </row>
-    <row r="360" spans="1:8" ht="179.35" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:8" ht="130.44999999999999" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>1437</v>
       </c>
@@ -57214,14 +57744,14 @@
       <c r="E360">
         <v>437</v>
       </c>
-      <c r="F360" s="14" t="s">
+      <c r="F360" s="13" t="s">
         <v>2122</v>
       </c>
       <c r="G360">
         <v>507</v>
       </c>
     </row>
-    <row r="361" spans="1:8" ht="97.85" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:8" ht="48.9" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>1442</v>
       </c>
@@ -57237,7 +57767,7 @@
       <c r="E361">
         <v>966</v>
       </c>
-      <c r="F361" s="14" t="s">
+      <c r="F361" s="13" t="s">
         <v>2125</v>
       </c>
       <c r="G361">
@@ -57261,7 +57791,7 @@
         <v>2129</v>
       </c>
     </row>
-    <row r="363" spans="1:8" ht="407.55" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:8" ht="293.45" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>1534</v>
       </c>
@@ -57274,7 +57804,7 @@
       <c r="D363" t="s">
         <v>2131</v>
       </c>
-      <c r="F363" s="14" t="s">
+      <c r="F363" s="13" t="s">
         <v>2132</v>
       </c>
       <c r="G363">
@@ -57334,7 +57864,7 @@
       <c r="D366" t="s">
         <v>2141</v>
       </c>
-      <c r="F366" s="14" t="s">
+      <c r="F366" s="13" t="s">
         <v>2142</v>
       </c>
     </row>
@@ -57419,7 +57949,7 @@
       <c r="D371" t="s">
         <v>2161</v>
       </c>
-      <c r="F371" s="14" t="s">
+      <c r="F371" s="13" t="s">
         <v>2162</v>
       </c>
     </row>
@@ -57440,7 +57970,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="373" spans="1:8" ht="195.65" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:8" ht="130.44999999999999" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>870</v>
       </c>
@@ -57453,7 +57983,7 @@
       <c r="D373" t="s">
         <v>2166</v>
       </c>
-      <c r="F373" s="14" t="s">
+      <c r="F373" s="13" t="s">
         <v>2167</v>
       </c>
     </row>
@@ -57614,7 +58144,7 @@
         <v>431340</v>
       </c>
     </row>
-    <row r="382" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:8" ht="244.55" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>1033</v>
       </c>
@@ -57627,7 +58157,7 @@
       <c r="D382" t="s">
         <v>2189</v>
       </c>
-      <c r="F382" s="14" t="s">
+      <c r="F382" s="13" t="s">
         <v>2190</v>
       </c>
       <c r="H382">
@@ -57668,7 +58198,7 @@
         <v>2196</v>
       </c>
     </row>
-    <row r="385" spans="1:6" ht="48.9" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:6" ht="32.6" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>2197</v>
       </c>
@@ -57681,7 +58211,7 @@
       <c r="D385" t="s">
         <v>2199</v>
       </c>
-      <c r="F385" s="14" t="s">
+      <c r="F385" s="13" t="s">
         <v>2200</v>
       </c>
     </row>
@@ -57734,6 +58264,1673 @@
       </c>
       <c r="F388" t="s">
         <v>2212</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42377BAB-23BC-44C4-BB10-F0AC361713D0}">
+  <dimension ref="A1:I70"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.3" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>730</v>
+      </c>
+      <c r="B1" t="s">
+        <v>731</v>
+      </c>
+      <c r="C1" t="s">
+        <v>732</v>
+      </c>
+      <c r="D1" t="s">
+        <v>733</v>
+      </c>
+      <c r="E1" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1" t="s">
+        <v>735</v>
+      </c>
+      <c r="G1" t="s">
+        <v>736</v>
+      </c>
+      <c r="H1" t="s">
+        <v>737</v>
+      </c>
+      <c r="I1" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1523</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1524</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1525</v>
+      </c>
+      <c r="H2">
+        <v>597479</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1911</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1912</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1913</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1914</v>
+      </c>
+      <c r="H3">
+        <v>639255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2002</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2003</v>
+      </c>
+      <c r="H4">
+        <v>639255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1392</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1394</v>
+      </c>
+      <c r="H5">
+        <v>563200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1328</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1329</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1330</v>
+      </c>
+      <c r="H6">
+        <v>563198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>956</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>957</v>
+      </c>
+      <c r="D7" t="s">
+        <v>958</v>
+      </c>
+      <c r="F7" t="s">
+        <v>959</v>
+      </c>
+      <c r="H7">
+        <v>690362</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1355</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1356</v>
+      </c>
+      <c r="H8">
+        <v>708571</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1308</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1309</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2286</v>
+      </c>
+      <c r="H9">
+        <v>708785</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1401</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1402</v>
+      </c>
+      <c r="H10">
+        <v>708580</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1447</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1448</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1449</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1450</v>
+      </c>
+      <c r="H11">
+        <v>708696</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>899</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>900</v>
+      </c>
+      <c r="D12" t="s">
+        <v>901</v>
+      </c>
+      <c r="E12">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>902</v>
+      </c>
+      <c r="G12" t="s">
+        <v>903</v>
+      </c>
+      <c r="H12">
+        <v>708791</v>
+      </c>
+      <c r="I12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>899</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E13">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1121</v>
+      </c>
+      <c r="G13" t="s">
+        <v>903</v>
+      </c>
+      <c r="H13">
+        <v>708791</v>
+      </c>
+      <c r="I13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1757</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1758</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1759</v>
+      </c>
+      <c r="H14">
+        <v>379432</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1881</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1882</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1883</v>
+      </c>
+      <c r="H15">
+        <v>379432</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>1579</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1580</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1581</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1582</v>
+      </c>
+      <c r="H16">
+        <v>561749</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>1579</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1949</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1950</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1951</v>
+      </c>
+      <c r="H17">
+        <v>561749</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>1575</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1576</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1577</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1578</v>
+      </c>
+      <c r="G18">
+        <v>386.4</v>
+      </c>
+      <c r="H18">
+        <v>561750</v>
+      </c>
+      <c r="I18">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1575</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1947</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1948</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1578</v>
+      </c>
+      <c r="G19">
+        <v>386.4</v>
+      </c>
+      <c r="H19">
+        <v>561750</v>
+      </c>
+      <c r="I19">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>754</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>755</v>
+      </c>
+      <c r="D20" t="s">
+        <v>756</v>
+      </c>
+      <c r="F20" t="s">
+        <v>757</v>
+      </c>
+      <c r="G20" t="s">
+        <v>758</v>
+      </c>
+      <c r="H20">
+        <v>751793</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>754</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>755</v>
+      </c>
+      <c r="D21" t="s">
+        <v>756</v>
+      </c>
+      <c r="F21" t="s">
+        <v>757</v>
+      </c>
+      <c r="G21" t="s">
+        <v>758</v>
+      </c>
+      <c r="H21">
+        <v>751793</v>
+      </c>
+      <c r="I21">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>754</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F22" t="s">
+        <v>757</v>
+      </c>
+      <c r="G22" t="s">
+        <v>758</v>
+      </c>
+      <c r="H22">
+        <v>751793</v>
+      </c>
+      <c r="I22">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1548</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1549</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1550</v>
+      </c>
+      <c r="H23">
+        <v>751783</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2133</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2134</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1550</v>
+      </c>
+      <c r="H24">
+        <v>751783</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1337</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1338</v>
+      </c>
+      <c r="E25">
+        <v>2923</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1339</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1340</v>
+      </c>
+      <c r="H25">
+        <v>732771</v>
+      </c>
+      <c r="I25">
+        <v>5446</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1334</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1335</v>
+      </c>
+      <c r="H26">
+        <v>732772</v>
+      </c>
+      <c r="I26">
+        <v>5940</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1815</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1816</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1817</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1818</v>
+      </c>
+      <c r="H27">
+        <v>732651</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>919</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>920</v>
+      </c>
+      <c r="D28" t="s">
+        <v>921</v>
+      </c>
+      <c r="F28" t="s">
+        <v>922</v>
+      </c>
+      <c r="H28">
+        <v>732754</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>919</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F29" t="s">
+        <v>922</v>
+      </c>
+      <c r="H29">
+        <v>732754</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1156</v>
+      </c>
+      <c r="H30">
+        <v>799973</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E31">
+        <v>226</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1161</v>
+      </c>
+      <c r="H31">
+        <v>799974</v>
+      </c>
+      <c r="I31">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1413</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E32">
+        <v>679</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1415</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1416</v>
+      </c>
+      <c r="H32">
+        <v>799979</v>
+      </c>
+      <c r="I32">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2106</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2107</v>
+      </c>
+      <c r="E33">
+        <v>679</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1415</v>
+      </c>
+      <c r="G33">
+        <v>684</v>
+      </c>
+      <c r="H33">
+        <v>799979</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1409</v>
+      </c>
+      <c r="E34">
+        <v>1273</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1410</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1411</v>
+      </c>
+      <c r="H34">
+        <v>799980</v>
+      </c>
+      <c r="I34">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="211.95" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2103</v>
+      </c>
+      <c r="D35" t="s">
+        <v>2104</v>
+      </c>
+      <c r="E35">
+        <v>1273</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>2105</v>
+      </c>
+      <c r="G35">
+        <v>1232</v>
+      </c>
+      <c r="H35">
+        <v>799980</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1428</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E36">
+        <v>638</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1430</v>
+      </c>
+      <c r="G36" t="s">
+        <v>1431</v>
+      </c>
+      <c r="H36">
+        <v>799975</v>
+      </c>
+      <c r="I36">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1423</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1424</v>
+      </c>
+      <c r="E37">
+        <v>676</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1425</v>
+      </c>
+      <c r="G37" t="s">
+        <v>1426</v>
+      </c>
+      <c r="H37">
+        <v>799976</v>
+      </c>
+      <c r="I37">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1379</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E38">
+        <v>3363</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1381</v>
+      </c>
+      <c r="G38" t="s">
+        <v>1382</v>
+      </c>
+      <c r="H38">
+        <v>799977</v>
+      </c>
+      <c r="I38">
+        <v>2429</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="211.95" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1187</v>
+      </c>
+      <c r="E39">
+        <v>2103</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>1188</v>
+      </c>
+      <c r="G39" t="s">
+        <v>1189</v>
+      </c>
+      <c r="H39">
+        <v>799978</v>
+      </c>
+      <c r="I39">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1147</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1148</v>
+      </c>
+      <c r="H40">
+        <v>766822</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1560</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1561</v>
+      </c>
+      <c r="F41" t="s">
+        <v>1148</v>
+      </c>
+      <c r="H41">
+        <v>766822</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1541</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1542</v>
+      </c>
+      <c r="H42">
+        <v>775571</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>1583</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1584</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1585</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1586</v>
+      </c>
+      <c r="H43">
+        <v>749004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>1583</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1952</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1953</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1586</v>
+      </c>
+      <c r="H44">
+        <v>749004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>1853</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1854</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1855</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1856</v>
+      </c>
+      <c r="H45">
+        <v>802791</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1152</v>
+      </c>
+      <c r="H46">
+        <v>800858</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1593</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1594</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1595</v>
+      </c>
+      <c r="H47">
+        <v>776486</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1957</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1958</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1595</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>776486</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2050</v>
+      </c>
+      <c r="D49" t="s">
+        <v>2051</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1595</v>
+      </c>
+      <c r="H49">
+        <v>776486</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1264</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1265</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1266</v>
+      </c>
+      <c r="G50" t="s">
+        <v>1267</v>
+      </c>
+      <c r="H50">
+        <v>800957</v>
+      </c>
+      <c r="I50">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D51" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E51">
+        <v>1668</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1178</v>
+      </c>
+      <c r="G51" t="s">
+        <v>1179</v>
+      </c>
+      <c r="H51">
+        <v>800469</v>
+      </c>
+      <c r="I51">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1171</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E52">
+        <v>2054</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1173</v>
+      </c>
+      <c r="G52" t="s">
+        <v>1174</v>
+      </c>
+      <c r="H52">
+        <v>800468</v>
+      </c>
+      <c r="I52">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F53" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H53">
+        <v>801111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1492</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1493</v>
+      </c>
+      <c r="F54" t="s">
+        <v>1494</v>
+      </c>
+      <c r="H54">
+        <v>801112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1397</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1398</v>
+      </c>
+      <c r="H55">
+        <v>801113</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>1487</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1488</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1489</v>
+      </c>
+      <c r="F56" t="s">
+        <v>1490</v>
+      </c>
+      <c r="H56">
+        <v>801114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="342.35" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1535</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1536</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>1537</v>
+      </c>
+      <c r="G57" t="s">
+        <v>1538</v>
+      </c>
+      <c r="H57">
+        <v>833011</v>
+      </c>
+      <c r="I57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="407.55" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>2130</v>
+      </c>
+      <c r="D58" t="s">
+        <v>2131</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>2132</v>
+      </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
+      <c r="H58">
+        <v>833011</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>1992</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1993</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1994</v>
+      </c>
+      <c r="E59">
+        <v>694</v>
+      </c>
+      <c r="F59" t="s">
+        <v>1995</v>
+      </c>
+      <c r="G59" t="s">
+        <v>1996</v>
+      </c>
+      <c r="H59">
+        <v>561295</v>
+      </c>
+      <c r="I59">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>1451</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1453</v>
+      </c>
+      <c r="F60" t="s">
+        <v>1454</v>
+      </c>
+      <c r="H60">
+        <v>801064</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>879</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>880</v>
+      </c>
+      <c r="D61" t="s">
+        <v>881</v>
+      </c>
+      <c r="F61" t="s">
+        <v>882</v>
+      </c>
+      <c r="G61" t="s">
+        <v>883</v>
+      </c>
+      <c r="H61">
+        <v>800940</v>
+      </c>
+      <c r="I61">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>879</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1110</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1111</v>
+      </c>
+      <c r="G62" t="s">
+        <v>1112</v>
+      </c>
+      <c r="H62">
+        <v>800940</v>
+      </c>
+      <c r="I62">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>909</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>910</v>
+      </c>
+      <c r="D63" t="s">
+        <v>911</v>
+      </c>
+      <c r="F63" t="s">
+        <v>912</v>
+      </c>
+      <c r="G63" t="s">
+        <v>913</v>
+      </c>
+      <c r="H63">
+        <v>801117</v>
+      </c>
+      <c r="I63">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>909</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F64" t="s">
+        <v>912</v>
+      </c>
+      <c r="G64" t="s">
+        <v>913</v>
+      </c>
+      <c r="H64">
+        <v>801117</v>
+      </c>
+      <c r="I64">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>894</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>895</v>
+      </c>
+      <c r="D65" t="s">
+        <v>896</v>
+      </c>
+      <c r="F65" t="s">
+        <v>897</v>
+      </c>
+      <c r="G65" t="s">
+        <v>898</v>
+      </c>
+      <c r="H65">
+        <v>801118</v>
+      </c>
+      <c r="I65">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>894</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1118</v>
+      </c>
+      <c r="F66" t="s">
+        <v>897</v>
+      </c>
+      <c r="G66" t="s">
+        <v>898</v>
+      </c>
+      <c r="H66">
+        <v>801118</v>
+      </c>
+      <c r="I66">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>889</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>890</v>
+      </c>
+      <c r="D67" t="s">
+        <v>891</v>
+      </c>
+      <c r="F67" t="s">
+        <v>892</v>
+      </c>
+      <c r="G67" t="s">
+        <v>893</v>
+      </c>
+      <c r="H67">
+        <v>801120</v>
+      </c>
+      <c r="I67">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>889</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F68" t="s">
+        <v>892</v>
+      </c>
+      <c r="G68" t="s">
+        <v>893</v>
+      </c>
+      <c r="H68">
+        <v>801120</v>
+      </c>
+      <c r="I68">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>904</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>905</v>
+      </c>
+      <c r="D69" t="s">
+        <v>906</v>
+      </c>
+      <c r="F69" t="s">
+        <v>907</v>
+      </c>
+      <c r="G69" t="s">
+        <v>908</v>
+      </c>
+      <c r="H69">
+        <v>801119</v>
+      </c>
+      <c r="I69">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>904</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F70" t="s">
+        <v>907</v>
+      </c>
+      <c r="G70" t="s">
+        <v>908</v>
+      </c>
+      <c r="H70">
+        <v>801119</v>
+      </c>
+      <c r="I70">
+        <v>792</v>
       </c>
     </row>
   </sheetData>
@@ -57742,6 +59939,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E7250ABCEFE04E4F81F2FF355B5D3A72" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c4fbf0553577fb8bea420e2142f9add2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="275848a0-c1ca-4a5e-8d43-94d4f8137f47" xmlns:ns3="0f5832fc-360e-4f5c-a190-e0499fab6bfe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd54e855f3815561d97cebadeb96de36" ns2:_="" ns3:_="">
     <xsd:import namespace="275848a0-c1ca-4a5e-8d43-94d4f8137f47"/>
@@ -57996,16 +60202,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9775FBD-11B8-4C50-BB24-61D42C8FEE27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B76448A-2C1E-4633-A440-72D49127B031}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -58022,12 +60227,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9775FBD-11B8-4C50-BB24-61D42C8FEE27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>